<commit_message>
change zorder of lines in plot
</commit_message>
<xml_diff>
--- a/data/vehicle_types.xlsx
+++ b/data/vehicle_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steff\Documents\Studium - UW\PUBPOL 594 A - Economic Approaches To Environmental Management\Project\tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E9A397-EC27-42D7-A054-BAA38FC948E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE229BA3-A74F-49CB-9F86-FFEFBF0B25B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -791,10 +791,10 @@
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
+      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -925,7 +925,7 @@
         <v>2</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -976,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
@@ -1028,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -1080,7 +1080,7 @@
         <v>2</v>
       </c>
       <c r="S5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
@@ -1131,7 +1131,7 @@
         <v>2</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
@@ -1183,7 +1183,7 @@
         <v>2</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
@@ -1235,7 +1235,7 @@
         <v>2</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
@@ -1287,7 +1287,7 @@
         <v>2</v>
       </c>
       <c r="S9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -1337,7 +1337,7 @@
         <v>2</v>
       </c>
       <c r="S10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -1387,7 +1387,7 @@
         <v>2</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
@@ -1440,7 +1440,7 @@
         <v>2</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -1493,7 +1493,7 @@
         <v>2</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -1543,7 +1543,7 @@
         <v>2</v>
       </c>
       <c r="S14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -1593,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -1643,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="S16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
@@ -1696,7 +1696,7 @@
         <v>2</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
@@ -1748,7 +1748,7 @@
         <v>2</v>
       </c>
       <c r="S18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
@@ -1791,7 +1791,7 @@
         <v>2</v>
       </c>
       <c r="S19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
@@ -1834,7 +1834,7 @@
         <v>2</v>
       </c>
       <c r="S20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
@@ -1877,7 +1877,7 @@
         <v>2</v>
       </c>
       <c r="S21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
@@ -1929,7 +1929,7 @@
         <v>2</v>
       </c>
       <c r="S22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
@@ -1970,7 +1970,7 @@
         <v>2</v>
       </c>
       <c r="S23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
@@ -2013,7 +2013,7 @@
         <v>2</v>
       </c>
       <c r="S24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
@@ -2056,7 +2056,7 @@
         <v>2</v>
       </c>
       <c r="S25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
@@ -2094,7 +2094,7 @@
         <v>2</v>
       </c>
       <c r="S26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
@@ -2126,7 +2126,7 @@
         <v>2</v>
       </c>
       <c r="S27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
@@ -2158,7 +2158,7 @@
         <v>2</v>
       </c>
       <c r="S28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
@@ -2190,7 +2190,7 @@
         <v>2</v>
       </c>
       <c r="S29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
@@ -2222,7 +2222,7 @@
         <v>2</v>
       </c>
       <c r="S30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
@@ -2254,7 +2254,7 @@
         <v>2</v>
       </c>
       <c r="S31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
@@ -2286,7 +2286,7 @@
         <v>2</v>
       </c>
       <c r="S32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
@@ -2318,7 +2318,7 @@
         <v>2</v>
       </c>
       <c r="S33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
@@ -2350,7 +2350,7 @@
         <v>2</v>
       </c>
       <c r="S34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
@@ -2382,7 +2382,7 @@
         <v>2</v>
       </c>
       <c r="S35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
@@ -2414,7 +2414,7 @@
         <v>2</v>
       </c>
       <c r="S36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>